<commit_message>
[WIP] New Tarrid - [FIX] ShoreHandling products - [ADD] On app add line with shorehandling
</commit_message>
<xml_diff>
--- a/lct_tos_integration/product.xlsx
+++ b/lct_tos_integration/product.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Generic products" sheetId="1" state="visible" r:id="rId2"/>
@@ -1746,7 +1746,7 @@
     <t>special_handling_code_id</t>
   </si>
   <si>
-    <t>special_handling_code_id/id</t>
+    <t>service_id/id</t>
   </si>
   <si>
     <t>Special handling code Scanning 20'</t>
@@ -2035,7 +2035,7 @@
   </sheetPr>
   <dimension ref="A1:AB770"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -26652,8 +26652,8 @@
   </sheetPr>
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
[FEEDBACK] Remove sub_category from SHC products & derivated duplicates
</commit_message>
<xml_diff>
--- a/lct_tos_integration/product.xlsx
+++ b/lct_tos_integration/product.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16973" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16901" uniqueCount="1126">
   <si>
     <t>Generic product name</t>
   </si>
@@ -3315,24 +3315,6 @@
     <t>Special handling code CFS Local import 40'</t>
   </si>
   <si>
-    <t>Special handling code CFS Free zone 20'</t>
-  </si>
-  <si>
-    <t>Special handling code CFS Free zone 40'</t>
-  </si>
-  <si>
-    <t>Special handling code CFS Transit Sahel 20'</t>
-  </si>
-  <si>
-    <t>Special handling code CFS Transit Sahel 40'</t>
-  </si>
-  <si>
-    <t>Special handling code CFS Transit coastal 20'</t>
-  </si>
-  <si>
-    <t>Special handling code CFS Transit coastal 40'</t>
-  </si>
-  <si>
     <t>Special handling code Cleaning 20'</t>
   </si>
   <si>
@@ -3351,24 +3333,6 @@
     <t>Special handling code Customs Local import 40'</t>
   </si>
   <si>
-    <t>Special handling code Customs Free zone 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Customs Free zone 40'</t>
-  </si>
-  <si>
-    <t>Special handling code Customs Transit Sahel 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Customs Transit Sahel 40'</t>
-  </si>
-  <si>
-    <t>Special handling code Customs Transit coastal 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Customs Transit coastal 40'</t>
-  </si>
-  <si>
     <t>Special handling code Direct delivery 20'</t>
   </si>
   <si>
@@ -3394,24 +3358,6 @@
   </si>
   <si>
     <t>Special handling code Inspection Local import 40'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Free zone 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Free zone 40'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Transit Sahel 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Transit Sahel 40'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Transit coastal 20'</t>
-  </si>
-  <si>
-    <t>Special handling code Inspection Transit coastal 40'</t>
   </si>
   <si>
     <t>Special handling code Pre-trip inspection20'</t>
@@ -61859,10 +61805,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -62009,13 +61955,10 @@
         <v>1099</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>1094</v>
@@ -62023,16 +61966,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>1100</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>1097</v>
-      </c>
       <c r="C8" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>1094</v>
@@ -62040,16 +61980,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1097</v>
+        <v>1103</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>1094</v>
@@ -62057,16 +61994,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1097</v>
+        <v>1103</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>1094</v>
@@ -62074,16 +62008,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>1094</v>
@@ -62091,16 +62022,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>1094</v>
@@ -62108,10 +62036,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>20</v>
@@ -62122,10 +62050,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>40</v>
@@ -62136,10 +62064,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>20</v>
@@ -62150,10 +62078,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>40</v>
@@ -62164,16 +62092,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1109</v>
+        <v>1115</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>1094</v>
@@ -62181,16 +62106,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1109</v>
+        <v>1115</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>1094</v>
@@ -62198,16 +62120,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1109</v>
+        <v>1118</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>1094</v>
@@ -62215,16 +62134,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>1114</v>
+        <v>1119</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1109</v>
+        <v>1118</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>1094</v>
@@ -62232,16 +62148,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>1115</v>
+        <v>1120</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1109</v>
+        <v>1121</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>20</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>1094</v>
@@ -62249,16 +62162,13 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>1116</v>
+        <v>1122</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1109</v>
+        <v>1121</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>40</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>1094</v>
@@ -62266,10 +62176,10 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>1117</v>
+        <v>1123</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1118</v>
+        <v>1124</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>20</v>
@@ -62280,10 +62190,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>1119</v>
+        <v>1125</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1118</v>
+        <v>1124</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>40</v>
@@ -62292,276 +62202,24 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C25" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C26" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C28" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C29" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C30" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C31" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C32" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C33" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>1131</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="C34" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C35" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
-        <v>1135</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C37" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C38" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C39" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C41" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C42" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>1094</v>
-      </c>
-    </row>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[FEEDBACK] Remove 'Local Import' from SHC products
</commit_message>
<xml_diff>
--- a/lct_tos_integration/product.xlsx
+++ b/lct_tos_integration/product.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="421" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="296" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic products" sheetId="1" state="visible" r:id="rId2"/>
@@ -3306,13 +3306,13 @@
     <t>Special handling code Scanning 40'</t>
   </si>
   <si>
-    <t>Special handling code CFS Local import 20'</t>
+    <t>Special handling code CFS 20'</t>
   </si>
   <si>
     <t>CFS</t>
   </si>
   <si>
-    <t>Special handling code CFS Local import 40'</t>
+    <t>Special handling code CFS 40'</t>
   </si>
   <si>
     <t>Special handling code Cleaning 20'</t>
@@ -3324,13 +3324,13 @@
     <t>Special handling code Cleaning 40'</t>
   </si>
   <si>
-    <t>Special handling code Customs Local import 20'</t>
+    <t>Special handling code Customs 20'</t>
   </si>
   <si>
     <t>CUS</t>
   </si>
   <si>
-    <t>Special handling code Customs Local import 40'</t>
+    <t>Special handling code Customs 40'</t>
   </si>
   <si>
     <t>Special handling code Direct delivery 20'</t>
@@ -3351,13 +3351,13 @@
     <t>Special handling code Delivery for examination 40'</t>
   </si>
   <si>
-    <t>Special handling code Inspection Local import 20'</t>
+    <t>Special handling code Inspection 20'</t>
   </si>
   <si>
     <t>INS</t>
   </si>
   <si>
-    <t>Special handling code Inspection Local import 40'</t>
+    <t>Special handling code Inspection 40'</t>
   </si>
   <si>
     <t>Special handling code Pre-trip inspection20'</t>
@@ -61808,7 +61808,7 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>